<commit_message>
logger fifo change, document and structure update.
</commit_message>
<xml_diff>
--- a/document/系统设计文档说明.xlsx
+++ b/document/系统设计文档说明.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47304345-57C9-4EB2-8AAB-1613BD0B660A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="242" yWindow="109" windowWidth="14799" windowHeight="8011"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="I2C driver" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Plans" sheetId="2" r:id="rId1"/>
+    <sheet name="Driver" sheetId="1" r:id="rId2"/>
+    <sheet name="Linux细节" sheetId="3" r:id="rId3"/>
+    <sheet name="嵌入式Linux问题统计" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>bus驱动</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -204,26 +206,337 @@
   <si>
     <t>1.实现i2c驱动中的接口(probe, remove, suspend, resume等)                                        2.实现与应用层交互的接口(open，read，write，ioctl，close)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FM Version 1.0.0.7</t>
+  </si>
+  <si>
+    <t>I/O的堵塞非堵塞</t>
+  </si>
+  <si>
+    <t>Linux的I/O支持堵塞和非堵塞两种模式，可在open时设置，默认为堵塞的I/O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.扩展node模块为内部数据通讯管理模块，GUI由此模块管理
+2.删除UDP的支持，TCP，串口由服务器改为客户端，增加心跳包，维持单独可靠连接。
+3.上位机修改为服务器，增加心跳管理，对于图像的处理拆分成另一个应用，从此项目中移除。
+4.远程通讯协议重新构建，协议解析扩展，另外修改为异步通信，收到数据响应ack，有数据提交则通知服务器端
+</t>
+  </si>
+  <si>
+    <t>Linux System使用问题</t>
+  </si>
+  <si>
+    <t>ubuntu使用apt安装包提示 g++ : Depends: g++-5 (＞= 5.3.1-3~) but it is not going to be installed 缺少依赖包</t>
+  </si>
+  <si>
+    <t>/etc/apt/sources.list使用的源错误，可通过"lsb_release -a"  查看ubuntu版本，在通过网址https://mirrors.tuna.tsinghua.edu.cn/help/ubuntu/修改</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>系统找不到编译工具(如gcc，arm-linux-gnueabihf-gcc等)，或者在用户权限下能够正常找到，在root权限下无法找到</t>
+    </r>
+  </si>
+  <si>
+    <t>现象</t>
+  </si>
+  <si>
+    <t>解决办法</t>
+  </si>
+  <si>
+    <t>在用户权限下添加PATH对应路径为/etc/profile中的export PATH="xxx:&lt;添加gcc路径&gt;", 
+在root权限下PATH对应路径为/etc/environment中的PATH="xxx: &lt;添加gcc路径&gt;"</t>
+  </si>
+  <si>
+    <t>网络出错或者DNS异常，网络出错解决网络问题，DNS服务器异常的话解决办法:sudo vim /etc/resolv.conf
+内部添加如下DNS服务器
+nameserver 8.8.8.8
+nameserver 8.8.4.4
+再通过如下命令重启网络
+sudo /etc/init.d/networking restart  
+sudo /etc/init.d/network-manager restart</t>
+  </si>
+  <si>
+    <r>
+      <t>mkdir –p /lib/modules/&lt;linux-version&gt; #</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>如</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4.1.15
+depmod</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>modprobe加载显示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>xxx: disagrees about version of symbol module_layout</t>
+    </r>
+  </si>
+  <si>
+    <t>执行apt-get找不到资源包如Unable to locate package openssh-service</t>
+  </si>
+  <si>
+    <t>apt-get update
+apt-get upgrade</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>嵌入式</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Linux</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>系统启动时找不到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>proc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>路径下文件，命令执行异常</t>
+    </r>
+  </si>
+  <si>
+    <t>在/etc/init.d/rcS文件中加入
+mount –a
+mount -t proc proc /proc</t>
+  </si>
+  <si>
+    <r>
+      <t>apt-get update</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>报错</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Could not resolve host</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>当前路径下不存在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Makefile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>，或者使用小写的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>makefile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>，会导致以上错误</t>
+    </r>
+  </si>
+  <si>
+    <t>编译时报错: No rule to make target `/usr/kernel/hello/Makefile'. Stop.</t>
+  </si>
+  <si>
+    <t>sudo apt-get install lzop</t>
+  </si>
+  <si>
+    <t>执行时报错mq_open: Function not implemented</t>
+  </si>
+  <si>
+    <t>编译、执行失败问题</t>
+  </si>
+  <si>
+    <t>内核中不支持mq消息队列功能， 
+make menuconfig
+ 	General setup  ---&gt;
+[ ] POSIX Message Queues
+选中，重新编译</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t xml:space="preserve">编译时报错: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/bin/sh: 1: lzop: not found</t>
+    </r>
+  </si>
+  <si>
+    <t>驱动加载报错
+insmod:can't install '8188eu.ko', invalid module formate</t>
+  </si>
+  <si>
+    <t>内核编译版本和驱动不一致，需要重新编译驱动</t>
+  </si>
+  <si>
+    <t>文件再Windows平台打开后，导致CR/LF不一致</t>
+  </si>
+  <si>
+    <t>sudo apt-get install dos2unix
+find ./ -exec dos2unix {} \;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="SimSun"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="134"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -234,7 +547,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -242,11 +555,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -260,9 +625,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -270,12 +662,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -317,7 +712,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,9 +745,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -385,6 +797,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -560,25 +989,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="55.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="116">
+      <c r="A2" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D16" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="49.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="12.54296875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.6328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="49.36328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1"/>
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>44</v>
       </c>
@@ -592,13 +1050,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="4"/>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="4"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -607,7 +1065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29.05" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="29">
       <c r="A5" s="4"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -616,7 +1074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="4"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -625,10 +1083,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="58.1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="43.5">
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
@@ -645,7 +1103,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="58.1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="58">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -660,10 +1118,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="29.05" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="29">
       <c r="A13" s="4" t="s">
         <v>42</v>
       </c>
@@ -677,7 +1135,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29.05" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="29">
       <c r="A14" s="4"/>
       <c r="B14" s="2" t="s">
         <v>17</v>
@@ -686,7 +1144,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="4"/>
       <c r="B15" s="2" t="s">
         <v>20</v>
@@ -695,7 +1153,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="29.05" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="29">
       <c r="A16" s="4"/>
       <c r="B16" s="2" t="s">
         <v>18</v>
@@ -710,7 +1168,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29.05" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
         <v>23</v>
@@ -719,10 +1177,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="3"/>
     </row>
-    <row r="20" spans="1:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="14.5" customHeight="1">
       <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
@@ -730,19 +1188,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="4"/>
       <c r="B22" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="14.5" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>35</v>
       </c>
@@ -750,19 +1208,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="4"/>
       <c r="B24" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="4"/>
       <c r="B25" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="29.05" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="29">
       <c r="A26" s="4" t="s">
         <v>40</v>
       </c>
@@ -773,13 +1231,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="4"/>
       <c r="B27" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="4"/>
       <c r="B28" s="2" t="s">
         <v>39</v>
@@ -800,31 +1258,173 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="50.90625" style="5" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="29">
+      <c r="A2" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964B3870-B174-458A-A05F-0780E2A30EB8}">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="22.54296875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="69.7265625" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="42">
+      <c r="A2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28">
+      <c r="A3" s="12"/>
+      <c r="B3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="56">
+      <c r="A4" s="12"/>
+      <c r="B4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="112">
+      <c r="A5" s="12"/>
+      <c r="B5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.5">
+      <c r="A6" s="12"/>
+      <c r="B6" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" ht="42">
+      <c r="A7" s="12"/>
+      <c r="B7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" ht="28">
+      <c r="A8" s="12"/>
+      <c r="B8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" ht="42">
+      <c r="A9" s="13"/>
+      <c r="B9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" ht="28">
+      <c r="A10" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="12"/>
+      <c r="B11" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="70">
+      <c r="A12" s="13"/>
+      <c r="B12" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update for system document.
</commit_message>
<xml_diff>
--- a/document/系统设计文档说明.xlsx
+++ b/document/系统设计文档说明.xlsx
@@ -3,22 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47304345-57C9-4EB2-8AAB-1613BD0B660A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B69197-D339-4C9B-B5AB-7A67220FBCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plans" sheetId="2" r:id="rId1"/>
     <sheet name="Driver" sheetId="1" r:id="rId2"/>
-    <sheet name="Linux细节" sheetId="3" r:id="rId3"/>
-    <sheet name="嵌入式Linux问题统计" sheetId="4" r:id="rId4"/>
+    <sheet name="嵌入式Linux遇到问题统计" sheetId="4" r:id="rId3"/>
+    <sheet name="Linux知识" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>bus驱动</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -209,12 +209,6 @@
   </si>
   <si>
     <t>FM Version 1.0.0.7</t>
-  </si>
-  <si>
-    <t>I/O的堵塞非堵塞</t>
-  </si>
-  <si>
-    <t>Linux的I/O支持堵塞和非堵塞两种模式，可在open时设置，默认为堵塞的I/O</t>
   </si>
   <si>
     <t xml:space="preserve">1.扩展node模块为内部数据通讯管理模块，GUI由此模块管理
@@ -473,6 +467,61 @@
   <si>
     <t>sudo apt-get install dos2unix
 find ./ -exec dos2unix {} \;</t>
+  </si>
+  <si>
+    <t>命令</t>
+  </si>
+  <si>
+    <t>功能说明</t>
+  </si>
+  <si>
+    <t>readelf</t>
+  </si>
+  <si>
+    <t>用例</t>
+  </si>
+  <si>
+    <t>readelf -h &lt;file&gt; 读取头部信息
+readelf -S &lt;file&gt; 读取段位表信息
+readelf -V &lt;file&gt; 读取版本信息
+readelf -a &lt;file&gt; 读取所有信息</t>
+  </si>
+  <si>
+    <t>扩展</t>
+  </si>
+  <si>
+    <t>一般使用
+&lt;cmd&gt; -h -H获取使用命令信息
+&lt;cmd&gt; -v、-V获取版本信息</t>
+  </si>
+  <si>
+    <t>strip</t>
+  </si>
+  <si>
+    <t>去除可执行文件和共享库中不必要的符号信息的工具</t>
+  </si>
+  <si>
+    <t>用于阅读ELF格式文件的工具。它可以显示ELF文件的各个节（section）和段（segment）的信息，包括符号表、重定位表、动态链接信息等。</t>
+  </si>
+  <si>
+    <t>常用选项：
+-s 去除符号表和重定位表
+-d 去除调试信息
+-N 符号列表 去除指定的符号
+-K 符号列表 保留指定的符号
+-R 节列表 去除指定的节
+-p 设置文件的权限为只读
+-o 输出文件的名称</t>
+  </si>
+  <si>
+    <t>strace</t>
+  </si>
+  <si>
+    <t>用于跟踪程序的系统调用和信号的工具。它可以记录程序执行过程中的系统调用和信号，并输出相关的信息，包括系统调用的名称、参数、返回值等</t>
+  </si>
+  <si>
+    <t>strace [选项] 命令 [参数]
+strace -o &lt;file&gt; &lt;cmd&gt;</t>
   </si>
 </sst>
 </file>
@@ -623,9 +672,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -642,6 +688,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1002,13 +1051,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="116">
-      <c r="A2" s="5" t="s">
-        <v>50</v>
+      <c r="A2" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1037,7 +1086,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1"/>
     <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1051,13 +1100,13 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="4"/>
+      <c r="A3" s="10"/>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="4"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1066,7 +1115,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="29">
-      <c r="A5" s="4"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1075,7 +1124,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="4"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1087,7 +1136,7 @@
       <c r="A7" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="43.5">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1104,7 +1153,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="58">
-      <c r="A10" s="4"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1122,7 +1171,7 @@
       <c r="A11" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="29">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1136,7 +1185,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="29">
-      <c r="A14" s="4"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1145,7 +1194,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="4"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1154,7 +1203,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="29">
-      <c r="A16" s="4"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1169,7 +1218,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="29">
-      <c r="A17" s="4"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
@@ -1181,7 +1230,7 @@
       <c r="A18" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="14.5" customHeight="1">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1189,19 +1238,19 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.5" customHeight="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1209,19 +1258,19 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="4"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="4"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="29">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1232,13 +1281,13 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="4"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="2" t="s">
         <v>39</v>
       </c>
@@ -1259,164 +1308,135 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964B3870-B174-458A-A05F-0780E2A30EB8}">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="50.90625" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="29">
-      <c r="A2" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964B3870-B174-458A-A05F-0780E2A30EB8}">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="22.54296875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="45.453125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="69.7265625" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="6"/>
+    <col min="1" max="1" width="22.54296875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="69.7265625" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>56</v>
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="42">
       <c r="A2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28">
       <c r="A3" s="12"/>
-      <c r="B3" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>62</v>
+      <c r="B3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="56">
       <c r="A4" s="12"/>
-      <c r="B4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>57</v>
+      <c r="B4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="112">
       <c r="A5" s="12"/>
-      <c r="B5" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>58</v>
+      <c r="B5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="31.5">
       <c r="A6" s="12"/>
-      <c r="B6" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" ht="42">
       <c r="A7" s="12"/>
-      <c r="B7" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" ht="28">
       <c r="A8" s="12"/>
-      <c r="B8" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" ht="42">
       <c r="A9" s="13"/>
-      <c r="B9" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="7"/>
+      <c r="B9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" ht="28">
       <c r="A10" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="12"/>
-      <c r="B11" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>68</v>
+      <c r="B11" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="70">
       <c r="A12" s="13"/>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1427,4 +1447,79 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="11.7265625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="54.81640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="67.36328125" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="43.5">
+      <c r="A1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="58">
+      <c r="A3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="116">
+      <c r="A4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="43.5">
+      <c r="A5" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[manage]update for note and TCP protocol.
</commit_message>
<xml_diff>
--- a/document/系统设计文档说明.xlsx
+++ b/document/系统设计文档说明.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B69197-D339-4C9B-B5AB-7A67220FBCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A26C47B-9062-4A8B-959D-3DAF9540DBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plans" sheetId="2" r:id="rId1"/>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1453,7 +1453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>